<commit_message>
new results imported, run
</commit_message>
<xml_diff>
--- a/comparison/output/agg_score_stats.xlsx
+++ b/comparison/output/agg_score_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK4"/>
+  <dimension ref="A1:AK12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -628,182 +628,182 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>6565</t>
+          <t>297</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6557</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>292</t>
+          <t>65</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6549</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>292</t>
+          <t>64</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>23427</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>23627</t>
+          <t>3917</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>20573</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>54828</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>20573</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>184</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
           <t>3917</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>6549</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>23418</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>54828</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>10555</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>44175</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>29976</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>24490</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>44175</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>23491</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
         <is>
           <t>20574</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>54828</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>362</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>24490</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>10763</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
         <is>
           <t>20574</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>6554</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>23480</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>3917</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>145</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>147</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>54828</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>23491</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>20574</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>44201</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>10763</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>20574</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>292</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>24491</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>10627</t>
-        </is>
-      </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>44201</t>
-        </is>
-      </c>
-      <c r="AJ2" t="inlineStr">
-        <is>
-          <t>30045</t>
-        </is>
-      </c>
-      <c r="AK2" t="inlineStr">
-        <is>
-          <t>24491</t>
         </is>
       </c>
     </row>
@@ -815,182 +815,182 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5498</t>
+          <t>2982</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5454</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2955</t>
+          <t>221</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4736</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2953</t>
+          <t>200</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13211</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>14144</t>
+          <t>733</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>6305</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>28167</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>6305</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>1719</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>1161</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>102</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
           <t>733</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>6305</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>4735</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>12472</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>718</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
         <is>
           <t>28167</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>6305</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>735</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>4762</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>12670</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>733</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>1479</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>1474</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>28167</t>
-        </is>
-      </c>
       <c r="Z3" t="inlineStr">
         <is>
+          <t>7348</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>20496</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>17947</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>7038</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>323</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>20496</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
           <t>13411</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr">
+      <c r="AG3" t="inlineStr">
         <is>
           <t>6306</t>
         </is>
       </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>20449</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>3182</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>7038</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
         <is>
           <t>8450</t>
         </is>
       </c>
-      <c r="AE3" t="inlineStr">
+      <c r="AK3" t="inlineStr">
         <is>
           <t>6306</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>2958</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>7038</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>7710</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>20449</t>
-        </is>
-      </c>
-      <c r="AJ3" t="inlineStr">
-        <is>
-          <t>18171</t>
-        </is>
-      </c>
-      <c r="AK3" t="inlineStr">
-        <is>
-          <t>7038</t>
         </is>
       </c>
     </row>
@@ -1002,37 +1002,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>9135</t>
+          <t>4510</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>112</t>
+          <t>8409</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4406</t>
+          <t>1753</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>89</t>
+          <t>5841</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>4364</t>
+          <t>1047</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>18762</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>18514</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -1057,22 +1057,22 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2181</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>3190</t>
+          <t>1529</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>5945</t>
+          <t>800</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>16507</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -1082,12 +1082,12 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>89</t>
+          <t>5841</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>2357</t>
+          <t>1047</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
@@ -1097,22 +1097,22 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>2007</t>
+          <t>0</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>15488</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>2568</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>706</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
@@ -1122,62 +1122,1558 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
+          <t>9938</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>21241</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>24603</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>3572</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>2553</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>21241</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
           <t>19809</t>
         </is>
       </c>
-      <c r="AA4" t="inlineStr">
+      <c r="AG4" t="inlineStr">
         <is>
           <t>3572</t>
         </is>
       </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>154</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>22086</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>5557</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>3572</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
         <is>
           <t>10351</t>
         </is>
       </c>
-      <c r="AE4" t="inlineStr">
+      <c r="AK4" t="inlineStr">
         <is>
           <t>3572</t>
         </is>
       </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>4429</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>3572</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t>11492</t>
-        </is>
-      </c>
-      <c r="AI4" t="inlineStr">
-        <is>
-          <t>22086</t>
-        </is>
-      </c>
-      <c r="AJ4" t="inlineStr">
-        <is>
-          <t>25731</t>
-        </is>
-      </c>
-      <c r="AK4" t="inlineStr">
-        <is>
-          <t>3572</t>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>human_chess</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>15774</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>14499</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>511</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>13884</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>491</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>59017</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2107</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>65309</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>156588</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>65309</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>12296</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>3224</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>254</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>2107</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>13884</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>491</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>58382</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>615</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>156588</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>19830</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>135987</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>72901</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>67416</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>771</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>135987</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>59508</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>65315</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>16271</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>67416</t>
+        </is>
+      </c>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t>31765</t>
+        </is>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>65315</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>human_mane</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>3409</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2219</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>331</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2077</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>330</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>11496</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>366</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>1959</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>19640</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>1959</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>2820</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>525</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>366</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>2077</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>330</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>11353</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>142</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>19640</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>3110</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>16132</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>13573</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>2325</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>398</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>16132</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>11826</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>1962</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>3742</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>2325</t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>5852</t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t>1962</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>human_mane_to_mouse</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1875</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>609</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>14091</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>381</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>12079</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>4111</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>18539</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>138</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>535</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>1202</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>381</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>12078</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>1871</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>228</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>18539</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>1144</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>2102</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>4492</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>15293</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>2102</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>16190</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>13953</t>
+        </is>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t>2256</t>
+        </is>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>human_refseq</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>801</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>801</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>743</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>756</t>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AH8" t="inlineStr">
+        <is>
+          <t>743</t>
+        </is>
+      </c>
+      <c r="AI8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AJ8" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="AK8" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>human_to_chimp</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>34507</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>22171</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2104</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>12052</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>1851</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>82003</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>44928</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>175361</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>44928</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>24966</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>8556</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>985</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>12051</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>1851</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>71631</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>10119</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>253</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>175361</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>30744</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>141525</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>94055</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>44945</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>3092</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>141525</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>83854</t>
+        </is>
+      </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t>44932</t>
+        </is>
+      </c>
+      <c r="AH9" t="inlineStr">
+        <is>
+          <t>36361</t>
+        </is>
+      </c>
+      <c r="AI9" t="inlineStr">
+        <is>
+          <t>44945</t>
+        </is>
+      </c>
+      <c r="AJ9" t="inlineStr">
+        <is>
+          <t>46575</t>
+        </is>
+      </c>
+      <c r="AK9" t="inlineStr">
+        <is>
+          <t>44932</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>10481</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>16030</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1230</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>13491</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>1143</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>57845</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2698</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>49711</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>135393</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>49711</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>7555</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>2597</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>329</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>2696</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>13489</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>1141</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>55219</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>2539</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>135393</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>21323</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>112485</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>71336</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>52409</t>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>1585</t>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>112485</t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>58988</t>
+        </is>
+      </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>49739</t>
+        </is>
+      </c>
+      <c r="AH10" t="inlineStr">
+        <is>
+          <t>11648</t>
+        </is>
+      </c>
+      <c r="AI10" t="inlineStr">
+        <is>
+          <t>52409</t>
+        </is>
+      </c>
+      <c r="AJ10" t="inlineStr">
+        <is>
+          <t>26666</t>
+        </is>
+      </c>
+      <c r="AK10" t="inlineStr">
+        <is>
+          <t>49739</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>mouse_to_rat</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1201</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>751</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>519</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>152</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>324</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2767</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>1425</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>5869</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>1425</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>457</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>508</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>236</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>152</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>324</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>1973</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>599</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>195</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>5869</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>1259</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>3855</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>2919</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>1425</t>
+        </is>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>755</t>
+        </is>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t>3855</t>
+        </is>
+      </c>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>3091</t>
+        </is>
+      </c>
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t>1425</t>
+        </is>
+      </c>
+      <c r="AH11" t="inlineStr">
+        <is>
+          <t>1525</t>
+        </is>
+      </c>
+      <c r="AI11" t="inlineStr">
+        <is>
+          <t>1425</t>
+        </is>
+      </c>
+      <c r="AJ11" t="inlineStr">
+        <is>
+          <t>1353</t>
+        </is>
+      </c>
+      <c r="AK11" t="inlineStr">
+        <is>
+          <t>1425</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>rice</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>16366</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1299</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>4428</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>1297</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>4411</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>15719</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>20425</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>58929</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>20425</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>14919</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>1305</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>142</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>1297</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>4411</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>15700</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>58929</t>
+        </is>
+      </c>
+      <c r="Z12" t="inlineStr">
+        <is>
+          <t>3304</t>
+        </is>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>51044</t>
+        </is>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>17016</t>
+        </is>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>21125</t>
+        </is>
+      </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>4581</t>
+        </is>
+      </c>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t>51044</t>
+        </is>
+      </c>
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>20130</t>
+        </is>
+      </c>
+      <c r="AG12" t="inlineStr">
+        <is>
+          <t>20436</t>
+        </is>
+      </c>
+      <c r="AH12" t="inlineStr">
+        <is>
+          <t>20788</t>
+        </is>
+      </c>
+      <c r="AI12" t="inlineStr">
+        <is>
+          <t>21125</t>
+        </is>
+      </c>
+      <c r="AJ12" t="inlineStr">
+        <is>
+          <t>18363</t>
+        </is>
+      </c>
+      <c r="AK12" t="inlineStr">
+        <is>
+          <t>20436</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
modified to take better lifton score and regenerated results
</commit_message>
<xml_diff>
--- a/comparison/output/agg_score_stats.xlsx
+++ b/comparison/output/agg_score_stats.xlsx
@@ -561,62 +561,62 @@
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
+          <t>lifton_score&gt;liftoff_score</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>lifton_score=liftoff_score</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>lifton_score&gt;miniprot_score</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>lifton_score=miniprot_score</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>liftoff_score&gt;lifton_score</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>liftoff_score=lifton_score</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
           <t>liftoff_score&gt;miniprot_score</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>liftoff_score=miniprot_score</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>liftoff_score&gt;lifton_score</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>liftoff_score=lifton_score</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>miniprot_score&gt;lifton_score</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>miniprot_score=lifton_score</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>miniprot_score&gt;liftoff_score</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>miniprot_score=liftoff_score</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>miniprot_score&gt;lifton_score</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>miniprot_score=lifton_score</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>lifton_score&gt;liftoff_score</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>lifton_score=liftoff_score</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>lifton_score&gt;miniprot_score</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>lifton_score=miniprot_score</t>
         </is>
       </c>
     </row>
@@ -628,47 +628,47 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>297</t>
+          <t>300</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>6557</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>6549</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>23427</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>3917</t>
+          <t>10474</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>63</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>20573</t>
+          <t>43991</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -678,7 +678,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>20573</t>
+          <t>43991</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -693,27 +693,27 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>35</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>3917</t>
+          <t>10474</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>63</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>6549</t>
+          <t>0</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>0</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
@@ -728,17 +728,17 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>23418</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>0</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
@@ -748,62 +748,62 @@
       </c>
       <c r="Z2" t="inlineStr">
         <is>
+          <t>363</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>54465</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>10774</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>44054</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>54465</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
           <t>10555</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AG2" t="inlineStr">
         <is>
           <t>44175</t>
         </is>
       </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>29976</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>24490</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>44054</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
         <is>
           <t>98</t>
         </is>
       </c>
-      <c r="AE2" t="inlineStr">
+      <c r="AK2" t="inlineStr">
         <is>
           <t>44175</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>23491</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>20574</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>362</t>
-        </is>
-      </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>24490</t>
-        </is>
-      </c>
-      <c r="AJ2" t="inlineStr">
-        <is>
-          <t>10763</t>
-        </is>
-      </c>
-      <c r="AK2" t="inlineStr">
-        <is>
-          <t>20574</t>
         </is>
       </c>
     </row>
@@ -815,182 +815,182 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2982</t>
+          <t>3009</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5454</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>221</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>4736</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>13211</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>733</t>
+          <t>6175</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
+          <t>211</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>18764</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>28167</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>18764</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>1729</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>1169</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>6175</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>210</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>6305</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
         <is>
           <t>28167</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>6305</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>1719</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>1161</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>733</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>4735</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>12472</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>718</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>28167</t>
-        </is>
-      </c>
       <c r="Z3" t="inlineStr">
         <is>
+          <t>3221</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>24939</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>9186</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>18975</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>24939</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
           <t>7348</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr">
+      <c r="AG3" t="inlineStr">
         <is>
           <t>20496</t>
         </is>
       </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>17947</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>7038</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>18975</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
         <is>
           <t>323</t>
         </is>
       </c>
-      <c r="AE3" t="inlineStr">
+      <c r="AK3" t="inlineStr">
         <is>
           <t>20496</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>13411</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>6306</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>3182</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>7038</t>
-        </is>
-      </c>
-      <c r="AJ3" t="inlineStr">
-        <is>
-          <t>8450</t>
-        </is>
-      </c>
-      <c r="AK3" t="inlineStr">
-        <is>
-          <t>6306</t>
         </is>
       </c>
     </row>
@@ -1002,47 +1002,47 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4510</t>
+          <t>5550</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>8409</t>
+          <t>42</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1753</t>
+          <t>60</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>5841</t>
+          <t>41</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1047</t>
+          <t>57</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>18762</t>
+          <t>55</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>7954</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1482</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>3572</t>
+          <t>18597</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -1052,67 +1052,67 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>3572</t>
+          <t>18597</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2181</t>
+          <t>2593</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>1529</t>
+          <t>1943</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>800</t>
+          <t>1014</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>7953</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1479</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>5841</t>
+          <t>38</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>1047</t>
+          <t>56</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>15488</t>
+          <t>51</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>2568</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>706</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
@@ -1122,62 +1122,62 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
+          <t>7085</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>26551</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>13541</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>20079</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>26551</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
           <t>9938</t>
         </is>
       </c>
-      <c r="AA4" t="inlineStr">
+      <c r="AG4" t="inlineStr">
         <is>
           <t>21241</t>
         </is>
       </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>24603</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>3572</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>112</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>20079</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
         <is>
           <t>2553</t>
         </is>
       </c>
-      <c r="AE4" t="inlineStr">
+      <c r="AK4" t="inlineStr">
         <is>
           <t>21241</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>19809</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>3572</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t>5557</t>
-        </is>
-      </c>
-      <c r="AI4" t="inlineStr">
-        <is>
-          <t>3572</t>
-        </is>
-      </c>
-      <c r="AJ4" t="inlineStr">
-        <is>
-          <t>10351</t>
-        </is>
-      </c>
-      <c r="AK4" t="inlineStr">
-        <is>
-          <t>3572</t>
         </is>
       </c>
     </row>
@@ -1189,47 +1189,47 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>15774</t>
+          <t>15808</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>14499</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>511</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>13884</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>491</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>59017</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2107</t>
+          <t>16602</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>507</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>65309</t>
+          <t>123671</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -1239,42 +1239,42 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>65309</t>
+          <t>123671</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>12296</t>
+          <t>12316</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>3224</t>
+          <t>3228</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>254</t>
+          <t>264</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>2107</t>
+          <t>16602</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>507</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>13884</t>
+          <t>0</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>491</t>
+          <t>0</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
@@ -1289,17 +1289,17 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>58382</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>615</t>
+          <t>0</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
@@ -1309,62 +1309,62 @@
       </c>
       <c r="Z5" t="inlineStr">
         <is>
+          <t>16315</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>140273</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>32410</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>124178</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>140273</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
           <t>19830</t>
         </is>
       </c>
-      <c r="AA5" t="inlineStr">
+      <c r="AG5" t="inlineStr">
         <is>
           <t>135987</t>
         </is>
       </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>72901</t>
-        </is>
-      </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>67416</t>
-        </is>
-      </c>
-      <c r="AD5" t="inlineStr">
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>124178</t>
+        </is>
+      </c>
+      <c r="AJ5" t="inlineStr">
         <is>
           <t>771</t>
         </is>
       </c>
-      <c r="AE5" t="inlineStr">
+      <c r="AK5" t="inlineStr">
         <is>
           <t>135987</t>
-        </is>
-      </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>59508</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>65315</t>
-        </is>
-      </c>
-      <c r="AH5" t="inlineStr">
-        <is>
-          <t>16271</t>
-        </is>
-      </c>
-      <c r="AI5" t="inlineStr">
-        <is>
-          <t>67416</t>
-        </is>
-      </c>
-      <c r="AJ5" t="inlineStr">
-        <is>
-          <t>31765</t>
-        </is>
-      </c>
-      <c r="AK5" t="inlineStr">
-        <is>
-          <t>65315</t>
         </is>
       </c>
     </row>
@@ -1376,47 +1376,47 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3409</t>
+          <t>3416</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2219</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>331</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2077</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>330</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>11496</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>366</t>
+          <t>2585</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>327</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>1959</t>
+          <t>13310</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -1426,12 +1426,12 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>1959</t>
+          <t>13310</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2820</t>
+          <t>2822</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -1441,27 +1441,27 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>69</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>366</t>
+          <t>2585</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>327</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>2077</t>
+          <t>0</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>330</t>
+          <t>2</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
@@ -1476,17 +1476,17 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>11353</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>142</t>
+          <t>0</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
@@ -1496,62 +1496,62 @@
       </c>
       <c r="Z6" t="inlineStr">
         <is>
+          <t>3745</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>15895</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>6001</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>13637</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>15895</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
           <t>3110</t>
         </is>
       </c>
-      <c r="AA6" t="inlineStr">
+      <c r="AG6" t="inlineStr">
         <is>
           <t>16132</t>
         </is>
       </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>13573</t>
-        </is>
-      </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>2325</t>
-        </is>
-      </c>
-      <c r="AD6" t="inlineStr">
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>13637</t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
         <is>
           <t>398</t>
         </is>
       </c>
-      <c r="AE6" t="inlineStr">
+      <c r="AK6" t="inlineStr">
         <is>
           <t>16132</t>
-        </is>
-      </c>
-      <c r="AF6" t="inlineStr">
-        <is>
-          <t>11826</t>
-        </is>
-      </c>
-      <c r="AG6" t="inlineStr">
-        <is>
-          <t>1962</t>
-        </is>
-      </c>
-      <c r="AH6" t="inlineStr">
-        <is>
-          <t>3742</t>
-        </is>
-      </c>
-      <c r="AI6" t="inlineStr">
-        <is>
-          <t>2325</t>
-        </is>
-      </c>
-      <c r="AJ6" t="inlineStr">
-        <is>
-          <t>5852</t>
-        </is>
-      </c>
-      <c r="AK6" t="inlineStr">
-        <is>
-          <t>1962</t>
         </is>
       </c>
     </row>
@@ -1563,182 +1563,182 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1875</t>
+          <t>3195</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>609</t>
+          <t>13</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>14091</t>
+          <t>262</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>381</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>12079</t>
+          <t>261</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>4111</t>
+          <t>8</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
+          <t>544</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>12639</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>1884</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>18539</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>1884</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>211</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>589</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>2395</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>542</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>12636</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>259</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>93</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
+      <c r="Y7" t="inlineStr">
         <is>
           <t>18539</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>93</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>138</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>535</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>1202</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>381</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>12078</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>1871</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>228</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>2012</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>18539</t>
-        </is>
-      </c>
       <c r="Z7" t="inlineStr">
         <is>
+          <t>16090</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>2428</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>3747</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>14523</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>2428</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
           <t>1144</t>
         </is>
       </c>
-      <c r="AA7" t="inlineStr">
+      <c r="AG7" t="inlineStr">
         <is>
           <t>2102</t>
         </is>
       </c>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>4492</t>
-        </is>
-      </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>94</t>
-        </is>
-      </c>
-      <c r="AD7" t="inlineStr">
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>269</t>
+        </is>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>14523</t>
+        </is>
+      </c>
+      <c r="AJ7" t="inlineStr">
         <is>
           <t>15293</t>
         </is>
       </c>
-      <c r="AE7" t="inlineStr">
+      <c r="AK7" t="inlineStr">
         <is>
           <t>2102</t>
-        </is>
-      </c>
-      <c r="AF7" t="inlineStr">
-        <is>
-          <t>16190</t>
-        </is>
-      </c>
-      <c r="AG7" t="inlineStr">
-        <is>
-          <t>93</t>
-        </is>
-      </c>
-      <c r="AH7" t="inlineStr">
-        <is>
-          <t>13953</t>
-        </is>
-      </c>
-      <c r="AI7" t="inlineStr">
-        <is>
-          <t>94</t>
-        </is>
-      </c>
-      <c r="AJ7" t="inlineStr">
-        <is>
-          <t>2256</t>
-        </is>
-      </c>
-      <c r="AK7" t="inlineStr">
-        <is>
-          <t>93</t>
         </is>
       </c>
     </row>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>46</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1760,7 +1760,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1770,12 +1770,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1785,12 +1785,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>690</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>58</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1800,7 +1800,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>58</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1815,7 +1815,7 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>46</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1825,7 +1825,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>690</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1835,7 +1835,7 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>7</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
@@ -1850,7 +1850,7 @@
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
@@ -1870,7 +1870,7 @@
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>743</t>
         </is>
       </c>
       <c r="AA8" t="inlineStr">
@@ -1880,52 +1880,52 @@
       </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>46</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>748</t>
         </is>
       </c>
       <c r="AD8" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="AH8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="AI8" t="inlineStr">
+        <is>
+          <t>748</t>
+        </is>
+      </c>
+      <c r="AJ8" t="inlineStr">
+        <is>
           <t>743</t>
         </is>
       </c>
-      <c r="AE8" t="inlineStr">
+      <c r="AK8" t="inlineStr">
         <is>
           <t>58</t>
-        </is>
-      </c>
-      <c r="AF8" t="inlineStr">
-        <is>
-          <t>756</t>
-        </is>
-      </c>
-      <c r="AG8" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AH8" t="inlineStr">
-        <is>
-          <t>743</t>
-        </is>
-      </c>
-      <c r="AI8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AJ8" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="AK8" t="inlineStr">
-        <is>
-          <t>5</t>
         </is>
       </c>
     </row>
@@ -1937,182 +1937,182 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>34507</t>
+          <t>35207</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>22171</t>
+          <t>31</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2104</t>
+          <t>27</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>12052</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>1851</t>
+          <t>27</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>82003</t>
+          <t>127</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
+          <t>21967</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>1887</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>116139</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>175361</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>116139</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>25266</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>8746</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>1195</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>21967</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>1870</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
           <t>17</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>44928</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
         <is>
           <t>175361</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>44928</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>24966</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>8556</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>985</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>12051</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>1851</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="V9" t="inlineStr">
-        <is>
-          <t>71631</t>
-        </is>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>10119</t>
-        </is>
-      </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>253</t>
-        </is>
-      </c>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t>175361</t>
-        </is>
-      </c>
       <c r="Z9" t="inlineStr">
         <is>
+          <t>37104</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>138106</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>57181</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>118026</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>138106</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
           <t>30744</t>
         </is>
       </c>
-      <c r="AA9" t="inlineStr">
+      <c r="AG9" t="inlineStr">
         <is>
           <t>141525</t>
         </is>
       </c>
-      <c r="AB9" t="inlineStr">
-        <is>
-          <t>94055</t>
-        </is>
-      </c>
-      <c r="AC9" t="inlineStr">
-        <is>
-          <t>44945</t>
-        </is>
-      </c>
-      <c r="AD9" t="inlineStr">
+      <c r="AH9" t="inlineStr">
+        <is>
+          <t>154</t>
+        </is>
+      </c>
+      <c r="AI9" t="inlineStr">
+        <is>
+          <t>118026</t>
+        </is>
+      </c>
+      <c r="AJ9" t="inlineStr">
         <is>
           <t>3092</t>
         </is>
       </c>
-      <c r="AE9" t="inlineStr">
+      <c r="AK9" t="inlineStr">
         <is>
           <t>141525</t>
-        </is>
-      </c>
-      <c r="AF9" t="inlineStr">
-        <is>
-          <t>83854</t>
-        </is>
-      </c>
-      <c r="AG9" t="inlineStr">
-        <is>
-          <t>44932</t>
-        </is>
-      </c>
-      <c r="AH9" t="inlineStr">
-        <is>
-          <t>36361</t>
-        </is>
-      </c>
-      <c r="AI9" t="inlineStr">
-        <is>
-          <t>44945</t>
-        </is>
-      </c>
-      <c r="AJ9" t="inlineStr">
-        <is>
-          <t>46575</t>
-        </is>
-      </c>
-      <c r="AK9" t="inlineStr">
-        <is>
-          <t>44932</t>
         </is>
       </c>
     </row>
@@ -2124,47 +2124,47 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>10481</t>
+          <t>10605</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>16030</t>
+          <t>32</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1230</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>13491</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>1143</t>
+          <t>10</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>57845</t>
+          <t>17</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2698</t>
+          <t>18655</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>1208</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>49711</t>
+          <t>104876</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -2174,67 +2174,67 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>49711</t>
+          <t>104876</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>7555</t>
+          <t>7600</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2597</t>
+          <t>2638</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>329</t>
+          <t>367</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>2696</t>
+          <t>18653</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>1208</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>13489</t>
+          <t>24</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>1141</t>
+          <t>8</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>55219</t>
+          <t>9</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>2539</t>
+          <t>8</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Y10" t="inlineStr">
@@ -2244,62 +2244,62 @@
       </c>
       <c r="Z10" t="inlineStr">
         <is>
+          <t>11821</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>123531</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>29282</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>106084</t>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>123531</t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
           <t>21323</t>
         </is>
       </c>
-      <c r="AA10" t="inlineStr">
+      <c r="AG10" t="inlineStr">
         <is>
           <t>112485</t>
         </is>
       </c>
-      <c r="AB10" t="inlineStr">
-        <is>
-          <t>71336</t>
-        </is>
-      </c>
-      <c r="AC10" t="inlineStr">
-        <is>
-          <t>52409</t>
-        </is>
-      </c>
-      <c r="AD10" t="inlineStr">
+      <c r="AH10" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="AI10" t="inlineStr">
+        <is>
+          <t>106084</t>
+        </is>
+      </c>
+      <c r="AJ10" t="inlineStr">
         <is>
           <t>1585</t>
         </is>
       </c>
-      <c r="AE10" t="inlineStr">
+      <c r="AK10" t="inlineStr">
         <is>
           <t>112485</t>
-        </is>
-      </c>
-      <c r="AF10" t="inlineStr">
-        <is>
-          <t>58988</t>
-        </is>
-      </c>
-      <c r="AG10" t="inlineStr">
-        <is>
-          <t>49739</t>
-        </is>
-      </c>
-      <c r="AH10" t="inlineStr">
-        <is>
-          <t>11648</t>
-        </is>
-      </c>
-      <c r="AI10" t="inlineStr">
-        <is>
-          <t>52409</t>
-        </is>
-      </c>
-      <c r="AJ10" t="inlineStr">
-        <is>
-          <t>26666</t>
-        </is>
-      </c>
-      <c r="AK10" t="inlineStr">
-        <is>
-          <t>49739</t>
         </is>
       </c>
     </row>
@@ -2311,47 +2311,47 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1201</t>
+          <t>1498</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>751</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>519</t>
+          <t>26</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>152</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>324</t>
+          <t>26</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2767</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>652</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>402</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>1425</t>
+          <t>3271</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -2361,42 +2361,42 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>1425</t>
+          <t>3271</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>457</t>
+          <t>564</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>508</t>
+          <t>607</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>236</t>
+          <t>327</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>649</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>402</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>152</t>
+          <t>2</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>324</t>
+          <t>23</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
@@ -2406,22 +2406,22 @@
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>1973</t>
+          <t>20</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>599</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>195</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
@@ -2431,62 +2431,62 @@
       </c>
       <c r="Z11" t="inlineStr">
         <is>
+          <t>1923</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>3923</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>2149</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>3673</t>
+        </is>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t>3923</t>
+        </is>
+      </c>
+      <c r="AF11" t="inlineStr">
+        <is>
           <t>1259</t>
         </is>
       </c>
-      <c r="AA11" t="inlineStr">
+      <c r="AG11" t="inlineStr">
         <is>
           <t>3855</t>
         </is>
       </c>
-      <c r="AB11" t="inlineStr">
-        <is>
-          <t>2919</t>
-        </is>
-      </c>
-      <c r="AC11" t="inlineStr">
-        <is>
-          <t>1425</t>
-        </is>
-      </c>
-      <c r="AD11" t="inlineStr">
+      <c r="AH11" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="AI11" t="inlineStr">
+        <is>
+          <t>3673</t>
+        </is>
+      </c>
+      <c r="AJ11" t="inlineStr">
         <is>
           <t>755</t>
         </is>
       </c>
-      <c r="AE11" t="inlineStr">
+      <c r="AK11" t="inlineStr">
         <is>
           <t>3855</t>
-        </is>
-      </c>
-      <c r="AF11" t="inlineStr">
-        <is>
-          <t>3091</t>
-        </is>
-      </c>
-      <c r="AG11" t="inlineStr">
-        <is>
-          <t>1425</t>
-        </is>
-      </c>
-      <c r="AH11" t="inlineStr">
-        <is>
-          <t>1525</t>
-        </is>
-      </c>
-      <c r="AI11" t="inlineStr">
-        <is>
-          <t>1425</t>
-        </is>
-      </c>
-      <c r="AJ11" t="inlineStr">
-        <is>
-          <t>1353</t>
-        </is>
-      </c>
-      <c r="AK11" t="inlineStr">
-        <is>
-          <t>1425</t>
         </is>
       </c>
     </row>
@@ -2498,47 +2498,47 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16366</t>
+          <t>16375</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1299</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>4428</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1297</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>4411</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>15719</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>1999</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4431</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>20425</t>
+          <t>36121</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -2548,12 +2548,12 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>20425</t>
+          <t>36121</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>14919</t>
+          <t>14922</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -2563,27 +2563,27 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>142</t>
+          <t>148</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>1999</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4431</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>1297</t>
+          <t>0</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>4411</t>
+          <t>2</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
@@ -2598,17 +2598,17 @@
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>15700</t>
+          <t>1</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
@@ -2618,62 +2618,62 @@
       </c>
       <c r="Z12" t="inlineStr">
         <is>
+          <t>20808</t>
+        </is>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>38120</t>
+        </is>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>18374</t>
+        </is>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>40552</t>
+        </is>
+      </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t>38120</t>
+        </is>
+      </c>
+      <c r="AF12" t="inlineStr">
+        <is>
           <t>3304</t>
         </is>
       </c>
-      <c r="AA12" t="inlineStr">
+      <c r="AG12" t="inlineStr">
         <is>
           <t>51044</t>
         </is>
       </c>
-      <c r="AB12" t="inlineStr">
-        <is>
-          <t>17016</t>
-        </is>
-      </c>
-      <c r="AC12" t="inlineStr">
-        <is>
-          <t>21125</t>
-        </is>
-      </c>
-      <c r="AD12" t="inlineStr">
+      <c r="AH12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AI12" t="inlineStr">
+        <is>
+          <t>40552</t>
+        </is>
+      </c>
+      <c r="AJ12" t="inlineStr">
         <is>
           <t>4581</t>
         </is>
       </c>
-      <c r="AE12" t="inlineStr">
+      <c r="AK12" t="inlineStr">
         <is>
           <t>51044</t>
-        </is>
-      </c>
-      <c r="AF12" t="inlineStr">
-        <is>
-          <t>20130</t>
-        </is>
-      </c>
-      <c r="AG12" t="inlineStr">
-        <is>
-          <t>20436</t>
-        </is>
-      </c>
-      <c r="AH12" t="inlineStr">
-        <is>
-          <t>20788</t>
-        </is>
-      </c>
-      <c r="AI12" t="inlineStr">
-        <is>
-          <t>21125</t>
-        </is>
-      </c>
-      <c r="AJ12" t="inlineStr">
-        <is>
-          <t>18363</t>
-        </is>
-      </c>
-      <c r="AK12" t="inlineStr">
-        <is>
-          <t>20436</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
using aa score as lifton score
</commit_message>
<xml_diff>
--- a/comparison/output/agg_score_stats.xlsx
+++ b/comparison/output/agg_score_stats.xlsx
@@ -628,7 +628,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>102</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -658,17 +658,17 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>10474</t>
+          <t>10525</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>84</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>43991</t>
+          <t>44117</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -678,32 +678,32 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>43991</t>
+          <t>44117</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>58</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>30</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>14</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>10474</t>
+          <t>10525</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>84</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -748,22 +748,22 @@
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>363</t>
+          <t>186</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>54465</t>
+          <t>54642</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>10774</t>
+          <t>10627</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>44054</t>
+          <t>44201</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr">
@@ -773,7 +773,7 @@
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>54465</t>
+          <t>54642</t>
         </is>
       </c>
       <c r="AF2" t="inlineStr">
@@ -793,7 +793,7 @@
       </c>
       <c r="AI2" t="inlineStr">
         <is>
-          <t>44054</t>
+          <t>44201</t>
         </is>
       </c>
       <c r="AJ2" t="inlineStr">
@@ -815,152 +815,152 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3009</t>
+          <t>600</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>7105</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>246</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>20203</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>28167</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>20203</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>290</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>236</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>7105</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>245</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>6175</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>211</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>18764</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
         <is>
           <t>28167</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>18764</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>1729</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>1169</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>6175</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>28167</t>
-        </is>
-      </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>3221</t>
+          <t>849</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>24939</t>
+          <t>27308</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>9186</t>
+          <t>7710</t>
         </is>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>18975</t>
+          <t>20449</t>
         </is>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>10</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>24939</t>
+          <t>27308</t>
         </is>
       </c>
       <c r="AF3" t="inlineStr">
@@ -975,12 +975,12 @@
       </c>
       <c r="AH3" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AI3" t="inlineStr">
         <is>
-          <t>18975</t>
+          <t>20449</t>
         </is>
       </c>
       <c r="AJ3" t="inlineStr">
@@ -1002,152 +1002,152 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5550</t>
+          <t>2508</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>66</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>60</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>83</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>8931</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>1804</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>20282</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>33732</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>20282</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>897</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>943</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>668</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>8929</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>1799</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
           <t>55</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>7954</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>1482</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>18597</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
         <is>
           <t>33732</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>18597</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>2593</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>1943</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>1014</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>7953</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>1479</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>56</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>33732</t>
-        </is>
-      </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>7085</t>
+          <t>4388</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>26551</t>
+          <t>29213</t>
         </is>
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>13541</t>
+          <t>11492</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>20079</t>
+          <t>22086</t>
         </is>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>131</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>26551</t>
+          <t>29213</t>
         </is>
       </c>
       <c r="AF4" t="inlineStr">
@@ -1162,12 +1162,12 @@
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>112</t>
+          <t>154</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr">
         <is>
-          <t>20079</t>
+          <t>22086</t>
         </is>
       </c>
       <c r="AJ4" t="inlineStr">
@@ -1189,17 +1189,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>15808</t>
+          <t>502</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1209,27 +1209,27 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>16602</t>
+          <t>19639</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>507</t>
+          <t>681</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>123671</t>
+          <t>135760</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -1239,32 +1239,32 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>123671</t>
+          <t>135760</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>12316</t>
+          <t>222</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>3228</t>
+          <t>191</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>264</t>
+          <t>89</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>16602</t>
+          <t>19638</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>507</t>
+          <t>681</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -1284,17 +1284,17 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
@@ -1309,32 +1309,32 @@
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>16315</t>
+          <t>1183</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>140273</t>
+          <t>155399</t>
         </is>
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>32410</t>
+          <t>20140</t>
         </is>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>124178</t>
+          <t>136441</t>
         </is>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>140273</t>
+          <t>155399</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">
@@ -1349,12 +1349,12 @@
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AI5" t="inlineStr">
         <is>
-          <t>124178</t>
+          <t>136441</t>
         </is>
       </c>
       <c r="AJ5" t="inlineStr">
@@ -1376,7 +1376,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3416</t>
+          <t>122</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1401,22 +1401,22 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2585</t>
+          <t>3083</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>327</t>
+          <t>378</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>13310</t>
+          <t>16054</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -1426,32 +1426,32 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>13310</t>
+          <t>16054</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2822</t>
+          <t>77</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>525</t>
+          <t>27</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>18</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>2585</t>
+          <t>3083</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>327</t>
+          <t>378</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -1476,7 +1476,7 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
@@ -1496,32 +1496,32 @@
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>3745</t>
+          <t>502</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>15895</t>
+          <t>19137</t>
         </is>
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>6001</t>
+          <t>3205</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>13637</t>
+          <t>16432</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>15895</t>
+          <t>19137</t>
         </is>
       </c>
       <c r="AF6" t="inlineStr">
@@ -1536,12 +1536,12 @@
       </c>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AI6" t="inlineStr">
         <is>
-          <t>13637</t>
+          <t>16432</t>
         </is>
       </c>
       <c r="AJ6" t="inlineStr">
@@ -1563,47 +1563,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>3195</t>
+          <t>2323</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>37</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>262</t>
+          <t>298</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>36</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>261</t>
+          <t>296</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>544</t>
+          <t>722</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>12639</t>
+          <t>13219</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>1884</t>
+          <t>1946</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1613,69 +1613,69 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>1884</t>
+          <t>1946</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>211</t>
+          <t>149</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>589</t>
+          <t>391</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>2395</t>
+          <t>1783</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>542</t>
+          <t>716</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>12636</t>
+          <t>13212</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>29</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>259</t>
+          <t>290</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="Y7" t="inlineStr">
         <is>
           <t>18539</t>
@@ -1683,32 +1683,32 @@
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>16090</t>
+          <t>15825</t>
         </is>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>2428</t>
+          <t>2668</t>
         </is>
       </c>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>3747</t>
+          <t>3068</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>14523</t>
+          <t>15165</t>
         </is>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>46</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>2428</t>
+          <t>2668</t>
         </is>
       </c>
       <c r="AF7" t="inlineStr">
@@ -1723,12 +1723,12 @@
       </c>
       <c r="AH7" t="inlineStr">
         <is>
-          <t>269</t>
+          <t>306</t>
         </is>
       </c>
       <c r="AI7" t="inlineStr">
         <is>
-          <t>14523</t>
+          <t>15165</t>
         </is>
       </c>
       <c r="AJ7" t="inlineStr">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>17</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1785,7 +1785,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>690</t>
+          <t>719</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1815,7 +1815,7 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>17</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1825,7 +1825,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>690</t>
+          <t>719</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1880,12 +1880,12 @@
       </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>17</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>748</t>
+          <t>777</t>
         </is>
       </c>
       <c r="AD8" t="inlineStr">
@@ -1915,7 +1915,7 @@
       </c>
       <c r="AI8" t="inlineStr">
         <is>
-          <t>748</t>
+          <t>777</t>
         </is>
       </c>
       <c r="AJ8" t="inlineStr">
@@ -1937,152 +1937,152 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>35207</t>
+          <t>6259</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>52</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>53</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>157</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>28884</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2420</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>137565</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>175361</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>137565</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>3812</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>1808</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>639</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>28884</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>2400</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
           <t>24</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>127</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>21967</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>1887</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>116139</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>148</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
         <is>
           <t>175361</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>116139</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>25266</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>8746</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>1195</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>21967</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>1870</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="V9" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t>175361</t>
-        </is>
-      </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>37104</t>
+          <t>8711</t>
         </is>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>138106</t>
+          <t>166449</t>
         </is>
       </c>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>57181</t>
+          <t>35167</t>
         </is>
       </c>
       <c r="AC9" t="inlineStr">
         <is>
-          <t>118026</t>
+          <t>139985</t>
         </is>
       </c>
       <c r="AD9" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>201</t>
         </is>
       </c>
       <c r="AE9" t="inlineStr">
         <is>
-          <t>138106</t>
+          <t>166449</t>
         </is>
       </c>
       <c r="AF9" t="inlineStr">
@@ -2097,12 +2097,12 @@
       </c>
       <c r="AH9" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>209</t>
         </is>
       </c>
       <c r="AI9" t="inlineStr">
         <is>
-          <t>118026</t>
+          <t>139985</t>
         </is>
       </c>
       <c r="AJ9" t="inlineStr">
@@ -2124,47 +2124,47 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>10605</t>
+          <t>1299</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>43</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>29</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>14</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>26</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>18655</t>
+          <t>20869</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1208</t>
+          <t>1420</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>104876</t>
+          <t>111745</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -2174,47 +2174,47 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>104876</t>
+          <t>111745</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>7600</t>
+          <t>728</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2638</t>
+          <t>413</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>367</t>
+          <t>158</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>18653</t>
+          <t>20867</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>1208</t>
+          <t>1413</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>22</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>7</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -2224,12 +2224,12 @@
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
@@ -2244,32 +2244,32 @@
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>11821</t>
+          <t>2724</t>
         </is>
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>123531</t>
+          <t>132614</t>
         </is>
       </c>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>29282</t>
+          <t>22188</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr">
         <is>
-          <t>106084</t>
+          <t>113165</t>
         </is>
       </c>
       <c r="AD10" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>55</t>
         </is>
       </c>
       <c r="AE10" t="inlineStr">
         <is>
-          <t>123531</t>
+          <t>132614</t>
         </is>
       </c>
       <c r="AF10" t="inlineStr">
@@ -2284,12 +2284,12 @@
       </c>
       <c r="AH10" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>40</t>
         </is>
       </c>
       <c r="AI10" t="inlineStr">
         <is>
-          <t>106084</t>
+          <t>113165</t>
         </is>
       </c>
       <c r="AJ10" t="inlineStr">
@@ -2311,152 +2311,152 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1498</t>
+          <t>990</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>11</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>26</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>847</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>488</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>3483</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>5869</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>3483</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>347</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>406</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>237</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>842</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>486</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>652</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>402</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>3271</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
         <is>
           <t>5869</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>3271</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>564</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>607</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>327</t>
-        </is>
-      </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>649</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>402</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="T11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="V11" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="W11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="X11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Y11" t="inlineStr">
-        <is>
-          <t>5869</t>
-        </is>
-      </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>1923</t>
+          <t>1503</t>
         </is>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>3923</t>
+          <t>4330</t>
         </is>
       </c>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>2149</t>
+          <t>1840</t>
         </is>
       </c>
       <c r="AC11" t="inlineStr">
         <is>
-          <t>3673</t>
+          <t>3971</t>
         </is>
       </c>
       <c r="AD11" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>36</t>
         </is>
       </c>
       <c r="AE11" t="inlineStr">
         <is>
-          <t>3923</t>
+          <t>4330</t>
         </is>
       </c>
       <c r="AF11" t="inlineStr">
@@ -2471,12 +2471,12 @@
       </c>
       <c r="AH11" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>58</t>
         </is>
       </c>
       <c r="AI11" t="inlineStr">
         <is>
-          <t>3673</t>
+          <t>3971</t>
         </is>
       </c>
       <c r="AJ11" t="inlineStr">
@@ -2498,7 +2498,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16375</t>
+          <t>67</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2508,7 +2508,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -2518,27 +2518,27 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>9</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1999</t>
+          <t>3293</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>4431</t>
+          <t>4538</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>36121</t>
+          <t>51018</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -2548,32 +2548,32 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>36121</t>
+          <t>51018</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>14922</t>
+          <t>21</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>1305</t>
+          <t>17</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>148</t>
+          <t>29</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>1999</t>
+          <t>3287</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>4431</t>
+          <t>4538</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -2583,7 +2583,7 @@
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
@@ -2593,12 +2593,12 @@
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
@@ -2608,7 +2608,7 @@
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
@@ -2618,32 +2618,32 @@
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>20808</t>
+          <t>4608</t>
         </is>
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>38120</t>
+          <t>54311</t>
         </is>
       </c>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>18374</t>
+          <t>3354</t>
         </is>
       </c>
       <c r="AC12" t="inlineStr">
         <is>
-          <t>40552</t>
+          <t>55556</t>
         </is>
       </c>
       <c r="AD12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>10</t>
         </is>
       </c>
       <c r="AE12" t="inlineStr">
         <is>
-          <t>38120</t>
+          <t>54311</t>
         </is>
       </c>
       <c r="AF12" t="inlineStr">
@@ -2658,12 +2658,12 @@
       </c>
       <c r="AH12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>19</t>
         </is>
       </c>
       <c r="AI12" t="inlineStr">
         <is>
-          <t>40552</t>
+          <t>55556</t>
         </is>
       </c>
       <c r="AJ12" t="inlineStr">

</xml_diff>